<commit_message>
link raw data files for Samples V11D01-384_A1,C1,D1, perform loupe alignment, and run spaceranger and results from spaceranger output
</commit_message>
<xml_diff>
--- a/raw-data/sample_info/visium-mastersheet.xlsx
+++ b/raw-data/sample_info/visium-mastersheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/var/folders/ky/wr2b0hfd37z07ng_j240xh1w0000gq/T/ch.sudo.cyberduck/editor-ad34f131-aeef-4eb2-acae-021e6d889f31/dcs04/lieber/marmaypag/spatialNac_LIBD4125/spatial_NAc/raw-data/sample_info/-911599233/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/var/folders/ky/wr2b0hfd37z07ng_j240xh1w0000gq/T/fz3temp-2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4617339-53E1-2740-9919-D68C639441F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C2E178B-974E-464C-B4F1-DE5C22E4FE9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="739" uniqueCount="361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="793" uniqueCount="387">
   <si>
     <t>Sample #</t>
   </si>
@@ -1126,6 +1126,84 @@
   </si>
   <si>
     <t>Br2743-Left</t>
+  </si>
+  <si>
+    <t>73v_NAc_SVB</t>
+  </si>
+  <si>
+    <t>Hs_Br3942</t>
+  </si>
+  <si>
+    <t>V13M06-379</t>
+  </si>
+  <si>
+    <t>SI-TT-C6</t>
+  </si>
+  <si>
+    <t>ACGACTACCA</t>
+  </si>
+  <si>
+    <t>ACGACCCTAA</t>
+  </si>
+  <si>
+    <t>TTAGGGTCGT</t>
+  </si>
+  <si>
+    <t>74v_NAc_SVB</t>
+  </si>
+  <si>
+    <t>SI-TT-H4</t>
+  </si>
+  <si>
+    <t>AGTTTCCTGG</t>
+  </si>
+  <si>
+    <t>TGCCACACAG</t>
+  </si>
+  <si>
+    <t>CTGTGTGGCA</t>
+  </si>
+  <si>
+    <t>75v_NAc_SVB</t>
+  </si>
+  <si>
+    <t>SI-TT-A5</t>
+  </si>
+  <si>
+    <t>GTAGCCCTGT</t>
+  </si>
+  <si>
+    <t>GAGCATCTAT</t>
+  </si>
+  <si>
+    <t>ATAGATGCTC</t>
+  </si>
+  <si>
+    <t>76v_NAc_SVB</t>
+  </si>
+  <si>
+    <t>SI-TT-B5</t>
+  </si>
+  <si>
+    <t>TCGGCTCTAC</t>
+  </si>
+  <si>
+    <t>CCGATGGTCT</t>
+  </si>
+  <si>
+    <t>AGACCATCGG</t>
+  </si>
+  <si>
+    <t>78v_NAc_SVB</t>
+  </si>
+  <si>
+    <t>Hs_Br8667</t>
+  </si>
+  <si>
+    <t>V13M13-362</t>
+  </si>
+  <si>
+    <t>79v_NAc_SVB</t>
   </si>
 </sst>
 </file>
@@ -1214,7 +1292,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1230,6 +1308,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1319,7 +1403,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="8">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1328,8 +1412,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1449,8 +1534,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="8" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="8">
+  <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1459,6 +1553,7 @@
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="7" builtinId="5"/>
+    <cellStyle name="Percent 2" xfId="8" xr:uid="{25A72E37-BEE6-164C-B6CF-6D8F7439DB32}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -2708,11 +2803,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y62"/>
+  <dimension ref="A1:Y68"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H1" sqref="H1"/>
+      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N76" sqref="N76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -6659,7 +6754,7 @@
         <v>617.40039999999999</v>
       </c>
       <c r="K55" s="47">
-        <f t="shared" ref="K55:K62" si="25">0.25*J55</f>
+        <f t="shared" ref="K55:K68" si="25">0.25*J55</f>
         <v>154.3501</v>
       </c>
       <c r="L55" s="32">
@@ -6694,7 +6789,7 @@
         <v>90</v>
       </c>
       <c r="V55" s="38">
-        <f t="shared" ref="V55:V62" si="27">((U55/100)*5000*60000)</f>
+        <f t="shared" ref="V55:V68" si="27">((U55/100)*5000*60000)</f>
         <v>270000000</v>
       </c>
     </row>
@@ -7200,6 +7295,438 @@
       <c r="V62" s="38">
         <f t="shared" si="27"/>
         <v>300000000</v>
+      </c>
+    </row>
+    <row r="63" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A63" s="32" t="s">
+        <v>361</v>
+      </c>
+      <c r="B63" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="C63" s="34" t="s">
+        <v>362</v>
+      </c>
+      <c r="D63" s="32" t="s">
+        <v>363</v>
+      </c>
+      <c r="E63" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="F63" s="35">
+        <v>15.64</v>
+      </c>
+      <c r="G63" s="32">
+        <v>16</v>
+      </c>
+      <c r="H63" s="36">
+        <v>7981.62</v>
+      </c>
+      <c r="I63" s="35">
+        <v>2</v>
+      </c>
+      <c r="J63" s="45">
+        <f>(H63*I63*40)/1000</f>
+        <v>638.52959999999996</v>
+      </c>
+      <c r="K63" s="45">
+        <f t="shared" si="25"/>
+        <v>159.63239999999999</v>
+      </c>
+      <c r="L63" s="32">
+        <v>15</v>
+      </c>
+      <c r="M63" s="32">
+        <v>456</v>
+      </c>
+      <c r="N63" s="36">
+        <v>5831.7</v>
+      </c>
+      <c r="O63" s="35">
+        <v>2</v>
+      </c>
+      <c r="P63" s="39">
+        <f>N63*O63</f>
+        <v>11663.4</v>
+      </c>
+      <c r="Q63" s="22" t="s">
+        <v>364</v>
+      </c>
+      <c r="R63" s="22" t="s">
+        <v>365</v>
+      </c>
+      <c r="S63" s="22" t="s">
+        <v>366</v>
+      </c>
+      <c r="T63" s="22" t="s">
+        <v>367</v>
+      </c>
+      <c r="U63" s="32">
+        <v>95</v>
+      </c>
+      <c r="V63" s="40">
+        <f t="shared" si="27"/>
+        <v>285000000</v>
+      </c>
+    </row>
+    <row r="64" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A64" s="32" t="s">
+        <v>368</v>
+      </c>
+      <c r="B64" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="C64" s="34" t="s">
+        <v>362</v>
+      </c>
+      <c r="D64" s="33" t="s">
+        <v>363</v>
+      </c>
+      <c r="E64" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="F64" s="35">
+        <v>15.3</v>
+      </c>
+      <c r="G64" s="32">
+        <v>15</v>
+      </c>
+      <c r="H64" s="36">
+        <v>6592.68</v>
+      </c>
+      <c r="I64" s="35">
+        <v>1</v>
+      </c>
+      <c r="J64" s="45">
+        <f>(H64*I64*40)/1000</f>
+        <v>263.7072</v>
+      </c>
+      <c r="K64" s="45">
+        <f t="shared" si="25"/>
+        <v>65.9268</v>
+      </c>
+      <c r="L64" s="32">
+        <v>17</v>
+      </c>
+      <c r="M64" s="32">
+        <v>459</v>
+      </c>
+      <c r="N64" s="36">
+        <v>4087.52</v>
+      </c>
+      <c r="O64" s="35">
+        <v>3</v>
+      </c>
+      <c r="P64" s="39">
+        <f t="shared" ref="P64:P68" si="28">N64*O64</f>
+        <v>12262.56</v>
+      </c>
+      <c r="Q64" s="22" t="s">
+        <v>369</v>
+      </c>
+      <c r="R64" s="22" t="s">
+        <v>370</v>
+      </c>
+      <c r="S64" s="22" t="s">
+        <v>371</v>
+      </c>
+      <c r="T64" s="22" t="s">
+        <v>372</v>
+      </c>
+      <c r="U64" s="32">
+        <v>90</v>
+      </c>
+      <c r="V64" s="40">
+        <f t="shared" si="27"/>
+        <v>270000000</v>
+      </c>
+    </row>
+    <row r="65" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A65" s="32" t="s">
+        <v>373</v>
+      </c>
+      <c r="B65" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="C65" s="34" t="s">
+        <v>362</v>
+      </c>
+      <c r="D65" s="33" t="s">
+        <v>363</v>
+      </c>
+      <c r="E65" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="F65" s="35">
+        <v>16.29</v>
+      </c>
+      <c r="G65" s="32">
+        <v>16</v>
+      </c>
+      <c r="H65" s="36">
+        <v>7232.42</v>
+      </c>
+      <c r="I65" s="35">
+        <v>1</v>
+      </c>
+      <c r="J65" s="45">
+        <f>(H65*I65*40)/1000</f>
+        <v>289.29679999999996</v>
+      </c>
+      <c r="K65" s="45">
+        <f t="shared" si="25"/>
+        <v>72.32419999999999</v>
+      </c>
+      <c r="L65" s="32">
+        <v>16</v>
+      </c>
+      <c r="M65" s="32">
+        <v>453</v>
+      </c>
+      <c r="N65" s="36">
+        <v>5603.41</v>
+      </c>
+      <c r="O65" s="35">
+        <v>2</v>
+      </c>
+      <c r="P65" s="39">
+        <f t="shared" si="28"/>
+        <v>11206.82</v>
+      </c>
+      <c r="Q65" s="22" t="s">
+        <v>374</v>
+      </c>
+      <c r="R65" s="22" t="s">
+        <v>375</v>
+      </c>
+      <c r="S65" s="22" t="s">
+        <v>376</v>
+      </c>
+      <c r="T65" s="22" t="s">
+        <v>377</v>
+      </c>
+      <c r="U65" s="32">
+        <v>85</v>
+      </c>
+      <c r="V65" s="40">
+        <f t="shared" si="27"/>
+        <v>255000000</v>
+      </c>
+    </row>
+    <row r="66" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A66" s="32" t="s">
+        <v>378</v>
+      </c>
+      <c r="B66" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="C66" s="34" t="s">
+        <v>362</v>
+      </c>
+      <c r="D66" s="33" t="s">
+        <v>363</v>
+      </c>
+      <c r="E66" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="F66" s="32">
+        <v>15.81</v>
+      </c>
+      <c r="G66" s="32">
+        <v>16</v>
+      </c>
+      <c r="H66" s="36">
+        <v>13327.41</v>
+      </c>
+      <c r="I66" s="35">
+        <v>1</v>
+      </c>
+      <c r="J66" s="45">
+        <f>(H66*I66*40)/1000</f>
+        <v>533.09640000000002</v>
+      </c>
+      <c r="K66" s="45">
+        <f t="shared" si="25"/>
+        <v>133.2741</v>
+      </c>
+      <c r="L66" s="32">
+        <v>15</v>
+      </c>
+      <c r="M66" s="32">
+        <v>487</v>
+      </c>
+      <c r="N66" s="36">
+        <v>5282.47</v>
+      </c>
+      <c r="O66" s="49">
+        <v>1</v>
+      </c>
+      <c r="P66" s="39">
+        <f t="shared" si="28"/>
+        <v>5282.47</v>
+      </c>
+      <c r="Q66" s="22" t="s">
+        <v>379</v>
+      </c>
+      <c r="R66" s="22" t="s">
+        <v>380</v>
+      </c>
+      <c r="S66" s="22" t="s">
+        <v>381</v>
+      </c>
+      <c r="T66" s="22" t="s">
+        <v>382</v>
+      </c>
+      <c r="U66" s="32">
+        <v>90</v>
+      </c>
+      <c r="V66" s="40">
+        <f t="shared" si="27"/>
+        <v>270000000</v>
+      </c>
+    </row>
+    <row r="67" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A67" s="32" t="s">
+        <v>383</v>
+      </c>
+      <c r="B67" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="C67" s="34" t="s">
+        <v>384</v>
+      </c>
+      <c r="D67" s="32" t="s">
+        <v>385</v>
+      </c>
+      <c r="E67" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="F67" s="50">
+        <v>15.33</v>
+      </c>
+      <c r="G67" s="46">
+        <v>15</v>
+      </c>
+      <c r="H67" s="36">
+        <v>7579.84</v>
+      </c>
+      <c r="I67" s="35">
+        <v>1</v>
+      </c>
+      <c r="J67" s="45">
+        <f>(H67*I67*40)/1000</f>
+        <v>303.1936</v>
+      </c>
+      <c r="K67" s="45">
+        <f t="shared" si="25"/>
+        <v>75.798400000000001</v>
+      </c>
+      <c r="L67" s="32">
+        <v>16</v>
+      </c>
+      <c r="M67" s="32">
+        <v>466</v>
+      </c>
+      <c r="N67" s="36">
+        <v>5719.38</v>
+      </c>
+      <c r="O67" s="35">
+        <v>4</v>
+      </c>
+      <c r="P67" s="39">
+        <f t="shared" si="28"/>
+        <v>22877.52</v>
+      </c>
+      <c r="Q67" s="22" t="s">
+        <v>277</v>
+      </c>
+      <c r="R67" s="22" t="s">
+        <v>278</v>
+      </c>
+      <c r="S67" s="22" t="s">
+        <v>279</v>
+      </c>
+      <c r="T67" s="22" t="s">
+        <v>280</v>
+      </c>
+      <c r="U67" s="32">
+        <v>85</v>
+      </c>
+      <c r="V67" s="51">
+        <f t="shared" si="27"/>
+        <v>255000000</v>
+      </c>
+    </row>
+    <row r="68" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A68" s="32" t="s">
+        <v>386</v>
+      </c>
+      <c r="B68" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="C68" s="34" t="s">
+        <v>384</v>
+      </c>
+      <c r="D68" s="32" t="s">
+        <v>385</v>
+      </c>
+      <c r="E68" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="F68" s="50">
+        <v>16.22</v>
+      </c>
+      <c r="G68" s="46">
+        <v>16</v>
+      </c>
+      <c r="H68" s="36">
+        <v>9431.33</v>
+      </c>
+      <c r="I68" s="35">
+        <v>1</v>
+      </c>
+      <c r="J68" s="45">
+        <f>(H68*I68*40)/1000</f>
+        <v>377.25319999999999</v>
+      </c>
+      <c r="K68" s="45">
+        <f t="shared" si="25"/>
+        <v>94.313299999999998</v>
+      </c>
+      <c r="L68" s="32">
+        <v>16</v>
+      </c>
+      <c r="M68" s="32">
+        <v>443</v>
+      </c>
+      <c r="N68" s="36">
+        <v>6269.72</v>
+      </c>
+      <c r="O68" s="35">
+        <v>4</v>
+      </c>
+      <c r="P68" s="39">
+        <f t="shared" si="28"/>
+        <v>25078.880000000001</v>
+      </c>
+      <c r="Q68" s="22" t="s">
+        <v>282</v>
+      </c>
+      <c r="R68" s="22" t="s">
+        <v>283</v>
+      </c>
+      <c r="S68" s="22" t="s">
+        <v>284</v>
+      </c>
+      <c r="T68" s="22" t="s">
+        <v>285</v>
+      </c>
+      <c r="U68" s="32">
+        <v>95</v>
+      </c>
+      <c r="V68" s="51">
+        <f t="shared" si="27"/>
+        <v>285000000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update visium excel sheet with most recent visium samples
</commit_message>
<xml_diff>
--- a/raw-data/sample_info/visium-mastersheet.xlsx
+++ b/raw-data/sample_info/visium-mastersheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11008"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/var/folders/ky/wr2b0hfd37z07ng_j240xh1w0000gq/T/fz3temp-2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/var/folders/ky/wr2b0hfd37z07ng_j240xh1w0000gq/T/ch.sudo.cyberduck/editor-ad16d467-b049-47e4-babf-1c61b2e94ee1/dcs04/lieber/marmaypag/spatialNac_LIBD4125/spatial_NAc/raw-data/sample_info/-1597990248/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C2E178B-974E-464C-B4F1-DE5C22E4FE9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF5EA370-BE8F-FC48-B85F-8EACBE224EEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="793" uniqueCount="387">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="820" uniqueCount="399">
   <si>
     <t>Sample #</t>
   </si>
@@ -1204,6 +1204,42 @@
   </si>
   <si>
     <t>79v_NAc_SVB</t>
+  </si>
+  <si>
+    <t>53v_NAc_SVB</t>
+  </si>
+  <si>
+    <t>Hs_Br6432</t>
+  </si>
+  <si>
+    <t>SI-TT-D6</t>
+  </si>
+  <si>
+    <t>CCCAGCTTCT</t>
+  </si>
+  <si>
+    <t>GACACCAAAC</t>
+  </si>
+  <si>
+    <t>GTTTGGTGTC</t>
+  </si>
+  <si>
+    <t>55v_NAc_SVB</t>
+  </si>
+  <si>
+    <t>SI-TT-B6</t>
+  </si>
+  <si>
+    <t>AATGCCATGA</t>
+  </si>
+  <si>
+    <t>TACGTAATGC</t>
+  </si>
+  <si>
+    <t>GCATTACGTA</t>
+  </si>
+  <si>
+    <t>56v_NAc_SVB</t>
   </si>
 </sst>
 </file>
@@ -1318,7 +1354,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -1402,6 +1438,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1414,7 +1459,7 @@
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1541,6 +1586,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2803,11 +2853,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y68"/>
+  <dimension ref="A1:Y71"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N76" sqref="N76"/>
+      <selection pane="bottomLeft" activeCell="A69" sqref="A69:V71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -6754,7 +6804,7 @@
         <v>617.40039999999999</v>
       </c>
       <c r="K55" s="47">
-        <f t="shared" ref="K55:K68" si="25">0.25*J55</f>
+        <f t="shared" ref="K55:K71" si="25">0.25*J55</f>
         <v>154.3501</v>
       </c>
       <c r="L55" s="32">
@@ -6789,7 +6839,7 @@
         <v>90</v>
       </c>
       <c r="V55" s="38">
-        <f t="shared" ref="V55:V68" si="27">((U55/100)*5000*60000)</f>
+        <f t="shared" ref="V55:V71" si="27">((U55/100)*5000*60000)</f>
         <v>270000000</v>
       </c>
     </row>
@@ -7326,7 +7376,7 @@
         <v>2</v>
       </c>
       <c r="J63" s="45">
-        <f>(H63*I63*40)/1000</f>
+        <f t="shared" ref="J63:J68" si="28">(H63*I63*40)/1000</f>
         <v>638.52959999999996</v>
       </c>
       <c r="K63" s="45">
@@ -7398,7 +7448,7 @@
         <v>1</v>
       </c>
       <c r="J64" s="45">
-        <f>(H64*I64*40)/1000</f>
+        <f t="shared" si="28"/>
         <v>263.7072</v>
       </c>
       <c r="K64" s="45">
@@ -7418,7 +7468,7 @@
         <v>3</v>
       </c>
       <c r="P64" s="39">
-        <f t="shared" ref="P64:P68" si="28">N64*O64</f>
+        <f t="shared" ref="P64:P68" si="29">N64*O64</f>
         <v>12262.56</v>
       </c>
       <c r="Q64" s="22" t="s">
@@ -7470,7 +7520,7 @@
         <v>1</v>
       </c>
       <c r="J65" s="45">
-        <f>(H65*I65*40)/1000</f>
+        <f t="shared" si="28"/>
         <v>289.29679999999996</v>
       </c>
       <c r="K65" s="45">
@@ -7490,7 +7540,7 @@
         <v>2</v>
       </c>
       <c r="P65" s="39">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>11206.82</v>
       </c>
       <c r="Q65" s="22" t="s">
@@ -7542,7 +7592,7 @@
         <v>1</v>
       </c>
       <c r="J66" s="45">
-        <f>(H66*I66*40)/1000</f>
+        <f t="shared" si="28"/>
         <v>533.09640000000002</v>
       </c>
       <c r="K66" s="45">
@@ -7562,7 +7612,7 @@
         <v>1</v>
       </c>
       <c r="P66" s="39">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>5282.47</v>
       </c>
       <c r="Q66" s="22" t="s">
@@ -7614,7 +7664,7 @@
         <v>1</v>
       </c>
       <c r="J67" s="45">
-        <f>(H67*I67*40)/1000</f>
+        <f t="shared" si="28"/>
         <v>303.1936</v>
       </c>
       <c r="K67" s="45">
@@ -7634,7 +7684,7 @@
         <v>4</v>
       </c>
       <c r="P67" s="39">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>22877.52</v>
       </c>
       <c r="Q67" s="22" t="s">
@@ -7686,7 +7736,7 @@
         <v>1</v>
       </c>
       <c r="J68" s="45">
-        <f>(H68*I68*40)/1000</f>
+        <f t="shared" si="28"/>
         <v>377.25319999999999</v>
       </c>
       <c r="K68" s="45">
@@ -7706,7 +7756,7 @@
         <v>4</v>
       </c>
       <c r="P68" s="39">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>25078.880000000001</v>
       </c>
       <c r="Q68" s="22" t="s">
@@ -7727,6 +7777,222 @@
       <c r="V68" s="51">
         <f t="shared" si="27"/>
         <v>285000000</v>
+      </c>
+    </row>
+    <row r="69" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A69" s="32" t="s">
+        <v>387</v>
+      </c>
+      <c r="B69" s="33" t="s">
+        <v>237</v>
+      </c>
+      <c r="C69" s="34" t="s">
+        <v>388</v>
+      </c>
+      <c r="D69" s="24" t="s">
+        <v>318</v>
+      </c>
+      <c r="E69" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="F69" s="35">
+        <v>15.48</v>
+      </c>
+      <c r="G69" s="32">
+        <v>16</v>
+      </c>
+      <c r="H69" s="36">
+        <v>5369.59</v>
+      </c>
+      <c r="I69" s="35">
+        <v>2</v>
+      </c>
+      <c r="J69" s="37">
+        <f>(H69*I69*40)/1000</f>
+        <v>429.56720000000001</v>
+      </c>
+      <c r="K69" s="37">
+        <f t="shared" si="25"/>
+        <v>107.3918</v>
+      </c>
+      <c r="L69" s="32">
+        <v>16</v>
+      </c>
+      <c r="M69" s="32">
+        <v>495</v>
+      </c>
+      <c r="N69" s="36">
+        <v>4567.83</v>
+      </c>
+      <c r="O69" s="35">
+        <v>3</v>
+      </c>
+      <c r="P69" s="42">
+        <f>N69*O69</f>
+        <v>13703.49</v>
+      </c>
+      <c r="Q69" s="22" t="s">
+        <v>389</v>
+      </c>
+      <c r="R69" s="22" t="s">
+        <v>390</v>
+      </c>
+      <c r="S69" s="22" t="s">
+        <v>391</v>
+      </c>
+      <c r="T69" s="22" t="s">
+        <v>392</v>
+      </c>
+      <c r="U69" s="32">
+        <v>99</v>
+      </c>
+      <c r="V69" s="38">
+        <f t="shared" si="27"/>
+        <v>297000000</v>
+      </c>
+    </row>
+    <row r="70" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A70" s="32" t="s">
+        <v>393</v>
+      </c>
+      <c r="B70" s="33" t="s">
+        <v>237</v>
+      </c>
+      <c r="C70" s="34" t="s">
+        <v>388</v>
+      </c>
+      <c r="D70" s="52" t="s">
+        <v>318</v>
+      </c>
+      <c r="E70" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="F70" s="35">
+        <v>16.5</v>
+      </c>
+      <c r="G70" s="32">
+        <v>17</v>
+      </c>
+      <c r="H70" s="36">
+        <v>4904.6400000000003</v>
+      </c>
+      <c r="I70" s="35">
+        <v>1</v>
+      </c>
+      <c r="J70" s="37">
+        <f>(H70*I70*40)/1000</f>
+        <v>196.18559999999999</v>
+      </c>
+      <c r="K70" s="37">
+        <f t="shared" si="25"/>
+        <v>49.046399999999998</v>
+      </c>
+      <c r="L70" s="32">
+        <v>17</v>
+      </c>
+      <c r="M70" s="32">
+        <v>449</v>
+      </c>
+      <c r="N70" s="36">
+        <v>2700.32</v>
+      </c>
+      <c r="O70" s="35">
+        <v>1</v>
+      </c>
+      <c r="P70" s="42">
+        <f>N70*O70</f>
+        <v>2700.32</v>
+      </c>
+      <c r="Q70" s="22" t="s">
+        <v>394</v>
+      </c>
+      <c r="R70" s="22" t="s">
+        <v>395</v>
+      </c>
+      <c r="S70" s="22" t="s">
+        <v>396</v>
+      </c>
+      <c r="T70" s="22" t="s">
+        <v>397</v>
+      </c>
+      <c r="U70" s="32">
+        <v>100</v>
+      </c>
+      <c r="V70" s="38">
+        <f t="shared" si="27"/>
+        <v>300000000</v>
+      </c>
+    </row>
+    <row r="71" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A71" s="32" t="s">
+        <v>398</v>
+      </c>
+      <c r="B71" s="33" t="s">
+        <v>237</v>
+      </c>
+      <c r="C71" s="34" t="s">
+        <v>388</v>
+      </c>
+      <c r="D71" s="53" t="s">
+        <v>318</v>
+      </c>
+      <c r="E71" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="F71" s="32">
+        <v>15.3</v>
+      </c>
+      <c r="G71" s="43">
+        <v>15</v>
+      </c>
+      <c r="H71" s="54">
+        <v>6040.9</v>
+      </c>
+      <c r="I71" s="35">
+        <v>1</v>
+      </c>
+      <c r="J71" s="37">
+        <f>(H71*I71*40)/1000</f>
+        <v>241.636</v>
+      </c>
+      <c r="K71" s="37">
+        <f t="shared" si="25"/>
+        <v>60.408999999999999</v>
+      </c>
+      <c r="L71" s="32">
+        <v>17</v>
+      </c>
+      <c r="M71" s="32">
+        <v>446</v>
+      </c>
+      <c r="N71" s="36">
+        <v>2315.35</v>
+      </c>
+      <c r="O71" s="44">
+        <v>1</v>
+      </c>
+      <c r="P71" s="42">
+        <f>N71*O71</f>
+        <v>2315.35</v>
+      </c>
+      <c r="Q71" s="22" t="s">
+        <v>364</v>
+      </c>
+      <c r="R71" s="22" t="s">
+        <v>365</v>
+      </c>
+      <c r="S71" s="22" t="s">
+        <v>366</v>
+      </c>
+      <c r="T71" s="22" t="s">
+        <v>367</v>
+      </c>
+      <c r="U71" s="32">
+        <v>90</v>
+      </c>
+      <c r="V71" s="38">
+        <f t="shared" si="27"/>
+        <v>270000000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>